<commit_message>
extra commit to incorporate knitted pdf
</commit_message>
<xml_diff>
--- a/HW4/Heritage R Model.xlsx
+++ b/HW4/Heritage R Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Documents\ETM 538\ETM538W2019\HW4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C2A9C6-21EE-4B47-BDB6-7FF8F8C2AFAE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3067A021-346D-4A95-8107-1902ED304DBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="391">
   <si>
     <t>Label</t>
   </si>
@@ -1205,6 +1205,30 @@
   </si>
   <si>
     <t>5+|O</t>
+  </si>
+  <si>
+    <t>26+ weeks|A</t>
+  </si>
+  <si>
+    <t>8-12 weeks|A</t>
+  </si>
+  <si>
+    <t>12-26 weeks|B</t>
+  </si>
+  <si>
+    <t>26+ weeks|B</t>
+  </si>
+  <si>
+    <t>8-12 weeks|B</t>
+  </si>
+  <si>
+    <t>26+ weeks|C</t>
+  </si>
+  <si>
+    <t>8-12 weeks|C</t>
+  </si>
+  <si>
+    <t>12-26 weeks|D</t>
   </si>
 </sst>
 </file>
@@ -1741,13 +1765,13 @@
         <v>294</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>6</v>
@@ -1776,15 +1800,15 @@
       </c>
       <c r="C4">
         <f>VLOOKUP(C$2&amp; "|" &amp;$B4,Charlson!$A$2:$F$21,6, FALSE)</f>
-        <v>0.37770762044704398</v>
+        <v>1.44231255090842E-2</v>
       </c>
       <c r="D4">
-        <f>VLOOKUP(D$2&amp; "|" &amp;$B4,Stay!$A$2:$F$58,6, FALSE)</f>
-        <v>2.0818132391194901E-4</v>
+        <f>VLOOKUP(D$2&amp; "|" &amp;$B4,Stay!$A$2:$F$66,6, FALSE)</f>
+        <v>2.0211779020577599E-5</v>
       </c>
       <c r="E4">
         <f>VLOOKUP(E$2&amp; "|" &amp;$B4,Condition!A2:F$225,6, FALSE)</f>
-        <v>0.11386912064613</v>
+        <v>1.7503400631820199E-3</v>
       </c>
       <c r="F4">
         <f>VLOOKUP(B4,'Risk Levels'!$A$2:$D$6, 4, FALSE)</f>
@@ -1792,11 +1816,11 @@
       </c>
       <c r="G4" s="7">
         <f>PRODUCT(C4:F4)*POWER(10,8)</f>
-        <v>687.1273361764346</v>
+        <v>3.9157964118299839E-2</v>
       </c>
       <c r="H4" s="4">
         <f>G4/G$9</f>
-        <v>0.4851941949669496</v>
+        <v>0.39694306641186522</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>20</v>
@@ -1814,15 +1838,15 @@
       </c>
       <c r="C5">
         <f>VLOOKUP(C$2&amp; "|" &amp;$B5,Charlson!$A$2:$F$21,6, FALSE)</f>
-        <v>0.45586816263977398</v>
+        <v>1.70662024861408E-2</v>
       </c>
       <c r="D5">
-        <f>VLOOKUP(D$2&amp; "|" &amp;$B5,Stay!$A$2:$F$58,6, FALSE)</f>
-        <v>3.78408037386714E-4</v>
+        <f>VLOOKUP(D$2&amp; "|" &amp;$B5,Stay!$A$2:$F$66,6, FALSE)</f>
+        <v>1.89204018693357E-5</v>
       </c>
       <c r="E5">
         <f>VLOOKUP(E$2&amp; "|" &amp;$B5,Condition!A3:F$225,6, FALSE)</f>
-        <v>0.101735000851418</v>
+        <v>1.5136321495468599E-3</v>
       </c>
       <c r="F5">
         <f>VLOOKUP(B5,'Risk Levels'!$A$2:$D$6, 4, FALSE)</f>
@@ -1830,11 +1854,11 @@
       </c>
       <c r="G5" s="7">
         <f t="shared" ref="G5" si="0">PRODUCT(C5:F5)*POWER(10,8)</f>
-        <v>143.87254939241072</v>
+        <v>4.0067802616540358E-3</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" ref="H5:H8" si="1">G5/G$9</f>
-        <v>0.10159125114819942</v>
+        <v>4.0616607101803114E-2</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>25</v>
@@ -1852,15 +1876,15 @@
       </c>
       <c r="C6">
         <f>VLOOKUP(C$2&amp; "|" &amp;$B6,Charlson!$A$2:$F$21,6, FALSE)</f>
-        <v>0.48612583400885501</v>
+        <v>1.80208268379373E-2</v>
       </c>
       <c r="D6">
-        <f>VLOOKUP(D$2&amp; "|" &amp;$B6,Stay!$A$2:$F$58,6, FALSE)</f>
-        <v>5.61202219866559E-4</v>
+        <f>VLOOKUP(D$2&amp; "|" &amp;$B6,Stay!$A$2:$F$66,6, FALSE)</f>
+        <v>6.2355802207395396E-5</v>
       </c>
       <c r="E6">
         <f>VLOOKUP(E$2&amp; "|" &amp;$B6,Condition!A4:F$225,6, FALSE)</f>
-        <v>9.8833946498721695E-2</v>
+        <v>4.3649061545176799E-4</v>
       </c>
       <c r="F6">
         <f>VLOOKUP(B6,'Risk Levels'!$A$2:$D$6, 4, FALSE)</f>
@@ -1868,11 +1892,11 @@
       </c>
       <c r="G6" s="7">
         <f t="shared" ref="G6:G8" si="2">PRODUCT(C6:F6)*POWER(10,8)</f>
-        <v>67.071131962584388</v>
+        <v>1.2200788882748095E-3</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="1"/>
-        <v>4.7360252117450596E-2</v>
+        <v>1.2367901806974989E-2</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>65</v>
@@ -1887,15 +1911,15 @@
       </c>
       <c r="C7">
         <f>VLOOKUP(C$2&amp; "|" &amp;$B7,Charlson!$A$2:$F$21,6, FALSE)</f>
-        <v>0.47047991713661003</v>
+        <v>2.1636551962251099E-2</v>
       </c>
       <c r="D7">
-        <f>VLOOKUP(D$2&amp; "|" &amp;$B7,Stay!$A$2:$F$58,6, FALSE)</f>
-        <v>2.87720105880999E-4</v>
+        <f>VLOOKUP(D$2&amp; "|" &amp;$B7,Stay!$A$2:$F$66,6, FALSE)</f>
+        <v>2.8772010588099901E-5</v>
       </c>
       <c r="E7">
         <f>VLOOKUP(E$2&amp; "|" &amp;$B7,Condition!A5:F$225,6, FALSE)</f>
-        <v>9.9551156634825597E-2</v>
+        <v>1.3522844976407E-3</v>
       </c>
       <c r="F7">
         <f>VLOOKUP(B7,'Risk Levels'!$A$2:$D$6, 4, FALSE)</f>
@@ -1903,11 +1927,11 @@
       </c>
       <c r="G7" s="7">
         <f t="shared" si="2"/>
-        <v>72.648338815532043</v>
+        <v>4.5383126263676176E-3</v>
       </c>
       <c r="H7" s="4">
         <f t="shared" si="1"/>
-        <v>5.129842812459065E-2</v>
+        <v>4.6004734178817237E-2</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>70</v>
@@ -1922,15 +1946,15 @@
       </c>
       <c r="C8">
         <f>VLOOKUP(C$2&amp; "|" &amp;$B8,Charlson!$A$2:$F$21,6, FALSE)</f>
-        <v>0.61355536836648705</v>
+        <v>3.6739454415862099E-2</v>
       </c>
       <c r="D8">
-        <f>VLOOKUP(D$2&amp; "|" &amp;$B8,Stay!$A$2:$F$58,6, FALSE)</f>
-        <v>9.28745761247543E-4</v>
+        <f>VLOOKUP(D$2&amp; "|" &amp;$B8,Stay!$A$2:$F$66,6, FALSE)</f>
+        <v>8.6394954534655202E-5</v>
       </c>
       <c r="E8">
         <f>VLOOKUP(E$2&amp; "|" &amp;$B8,Condition!A6:F$225,6, FALSE)</f>
-        <v>0.10885764271366601</v>
+        <v>2.1814726020000399E-3</v>
       </c>
       <c r="F8">
         <f>VLOOKUP(B8,'Risk Levels'!$A$2:$D$6, 4, FALSE)</f>
@@ -1938,11 +1962,11 @@
       </c>
       <c r="G8" s="7">
         <f t="shared" si="2"/>
-        <v>445.47099239214492</v>
+        <v>4.9725681610304572E-2</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="1"/>
-        <v>0.31455587364280957</v>
+        <v>0.50406769050053946</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>75</v>
@@ -1958,11 +1982,11 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7">
         <f>SUM(G4:G8)</f>
-        <v>1416.1903487391069</v>
+        <v>9.8648817504900871E-2</v>
       </c>
       <c r="H9" s="5">
         <f>SUM(H4:H8)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>30</v>
@@ -2203,10 +2227,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,7 +2239,7 @@
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2255,7 +2279,7 @@
         <v>0.52468166423854801</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2275,7 +2299,7 @@
         <v>0.45586816263977398</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2295,7 +2319,7 @@
         <v>1.70662024861408E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2315,7 +2339,7 @@
         <v>2.3839706355362998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2335,7 +2359,7 @@
         <v>0.49466857891126798</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2355,7 +2379,7 @@
         <v>0.48612583400885501</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2374,26 +2398,8 @@
       <c r="F8">
         <v>1.80208268379373E-2</v>
       </c>
-      <c r="L8" t="s">
-        <v>0</v>
-      </c>
-      <c r="M8" t="s">
-        <v>295</v>
-      </c>
-      <c r="N8" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>378</v>
       </c>
@@ -2412,29 +2418,8 @@
       <c r="F9">
         <v>1.1847602419405099E-3</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>7</v>
-      </c>
-      <c r="O9">
-        <v>27731</v>
-      </c>
-      <c r="P9">
-        <v>52853</v>
-      </c>
-      <c r="Q9">
-        <v>0.52468166423854801</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2453,29 +2438,9 @@
       <c r="F10">
         <v>0.50526527793762199</v>
       </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="8">
-        <v>43467</v>
-      </c>
-      <c r="N10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10">
-        <v>24094</v>
-      </c>
-      <c r="P10">
-        <v>52853</v>
-      </c>
-      <c r="Q10">
-        <v>0.45586816263977398</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2494,29 +2459,9 @@
       <c r="F11">
         <v>0.47047991713661003</v>
       </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="8">
-        <v>43528</v>
-      </c>
-      <c r="N11" t="s">
-        <v>7</v>
-      </c>
-      <c r="O11">
-        <v>902</v>
-      </c>
-      <c r="P11">
-        <v>52853</v>
-      </c>
-      <c r="Q11">
-        <v>1.70662024861408E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2535,29 +2480,8 @@
       <c r="F12">
         <v>2.1636551962251099E-2</v>
       </c>
-      <c r="K12">
-        <v>4</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" t="s">
-        <v>7</v>
-      </c>
-      <c r="O12">
-        <v>126</v>
-      </c>
-      <c r="P12">
-        <v>52853</v>
-      </c>
-      <c r="Q12">
-        <v>2.3839706355362998E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2576,29 +2500,8 @@
       <c r="F13">
         <v>2.6182529635170901E-3</v>
       </c>
-      <c r="K13">
-        <v>5</v>
-      </c>
-      <c r="L13" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13">
-        <v>7933</v>
-      </c>
-      <c r="P13">
-        <v>16037</v>
-      </c>
-      <c r="Q13">
-        <v>0.49466857891126798</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2617,29 +2520,9 @@
       <c r="F14">
         <v>0.346681353808938</v>
       </c>
-      <c r="K14">
-        <v>6</v>
-      </c>
-      <c r="L14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="8">
-        <v>43467</v>
-      </c>
-      <c r="N14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14">
-        <v>7796</v>
-      </c>
-      <c r="P14">
-        <v>16037</v>
-      </c>
-      <c r="Q14">
-        <v>0.48612583400885501</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2658,29 +2541,9 @@
       <c r="F15">
         <v>0.61355536836648705</v>
       </c>
-      <c r="K15">
-        <v>7</v>
-      </c>
-      <c r="L15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="8">
-        <v>43528</v>
-      </c>
-      <c r="N15" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15">
-        <v>289</v>
-      </c>
-      <c r="P15">
-        <v>16037</v>
-      </c>
-      <c r="Q15">
-        <v>1.80208268379373E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2699,29 +2562,8 @@
       <c r="F16">
         <v>3.6739454415862099E-2</v>
       </c>
-      <c r="K16">
-        <v>8</v>
-      </c>
-      <c r="L16" t="s">
-        <v>378</v>
-      </c>
-      <c r="M16" t="s">
-        <v>25</v>
-      </c>
-      <c r="N16" t="s">
-        <v>9</v>
-      </c>
-      <c r="O16">
-        <v>19</v>
-      </c>
-      <c r="P16">
-        <v>16037</v>
-      </c>
-      <c r="Q16">
-        <v>1.1847602419405099E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2740,29 +2582,8 @@
       <c r="F17">
         <v>3.02382340871293E-3</v>
       </c>
-      <c r="K17">
-        <v>9</v>
-      </c>
-      <c r="L17" t="s">
-        <v>10</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
-        <v>11</v>
-      </c>
-      <c r="O17">
-        <v>17561</v>
-      </c>
-      <c r="P17">
-        <v>34756</v>
-      </c>
-      <c r="Q17">
-        <v>0.50526527793762199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>379</v>
       </c>
@@ -2781,29 +2602,9 @@
       <c r="F18">
         <v>0.60618157049565302</v>
       </c>
-      <c r="K18">
-        <v>10</v>
-      </c>
-      <c r="L18" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="8">
-        <v>43467</v>
-      </c>
-      <c r="N18" t="s">
-        <v>11</v>
-      </c>
-      <c r="O18">
-        <v>16352</v>
-      </c>
-      <c r="P18">
-        <v>34756</v>
-      </c>
-      <c r="Q18">
-        <v>0.47047991713661003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>380</v>
       </c>
@@ -2822,29 +2623,9 @@
       <c r="F19">
         <v>0.37770762044704398</v>
       </c>
-      <c r="K19">
-        <v>11</v>
-      </c>
-      <c r="L19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="8">
-        <v>43528</v>
-      </c>
-      <c r="N19" t="s">
-        <v>11</v>
-      </c>
-      <c r="O19">
-        <v>752</v>
-      </c>
-      <c r="P19">
-        <v>34756</v>
-      </c>
-      <c r="Q19">
-        <v>2.1636551962251099E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>381</v>
       </c>
@@ -2863,29 +2644,8 @@
       <c r="F20">
         <v>1.44231255090842E-2</v>
       </c>
-      <c r="K20">
-        <v>12</v>
-      </c>
-      <c r="L20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" t="s">
-        <v>25</v>
-      </c>
-      <c r="N20" t="s">
-        <v>11</v>
-      </c>
-      <c r="O20">
-        <v>91</v>
-      </c>
-      <c r="P20">
-        <v>34756</v>
-      </c>
-      <c r="Q20">
-        <v>2.6182529635170901E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>382</v>
       </c>
@@ -2904,188 +2664,18 @@
       <c r="F21">
         <v>1.6876835482182301E-3</v>
       </c>
-      <c r="K21">
-        <v>13</v>
-      </c>
-      <c r="L21" t="s">
-        <v>12</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" t="s">
-        <v>13</v>
-      </c>
-      <c r="O21">
-        <v>16051</v>
-      </c>
-      <c r="P21">
-        <v>46299</v>
-      </c>
-      <c r="Q21">
-        <v>0.346681353808938</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K22">
-        <v>14</v>
-      </c>
-      <c r="L22" t="s">
-        <v>18</v>
-      </c>
-      <c r="M22" s="8">
-        <v>43467</v>
-      </c>
-      <c r="N22" t="s">
-        <v>13</v>
-      </c>
-      <c r="O22">
-        <v>28407</v>
-      </c>
-      <c r="P22">
-        <v>46299</v>
-      </c>
-      <c r="Q22">
-        <v>0.61355536836648705</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K23">
-        <v>15</v>
-      </c>
-      <c r="L23" t="s">
-        <v>23</v>
-      </c>
-      <c r="M23" s="8">
-        <v>43528</v>
-      </c>
-      <c r="N23" t="s">
-        <v>13</v>
-      </c>
-      <c r="O23">
-        <v>1701</v>
-      </c>
-      <c r="P23">
-        <v>46299</v>
-      </c>
-      <c r="Q23">
-        <v>3.6739454415862099E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K24">
-        <v>16</v>
-      </c>
-      <c r="L24" t="s">
-        <v>27</v>
-      </c>
-      <c r="M24" t="s">
-        <v>25</v>
-      </c>
-      <c r="N24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O24">
-        <v>140</v>
-      </c>
-      <c r="P24">
-        <v>46299</v>
-      </c>
-      <c r="Q24">
-        <v>3.02382340871293E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K25">
-        <v>17</v>
-      </c>
-      <c r="L25" t="s">
-        <v>379</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25" t="s">
-        <v>302</v>
-      </c>
-      <c r="O25">
-        <v>299915</v>
-      </c>
-      <c r="P25">
-        <v>494761</v>
-      </c>
-      <c r="Q25">
-        <v>0.60618157049565302</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K26">
-        <v>18</v>
-      </c>
-      <c r="L26" t="s">
-        <v>380</v>
-      </c>
-      <c r="M26" s="8">
-        <v>43467</v>
-      </c>
-      <c r="N26" t="s">
-        <v>302</v>
-      </c>
-      <c r="O26">
-        <v>186875</v>
-      </c>
-      <c r="P26">
-        <v>494761</v>
-      </c>
-      <c r="Q26">
-        <v>0.37770762044704398</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K27">
-        <v>19</v>
-      </c>
-      <c r="L27" t="s">
-        <v>381</v>
-      </c>
-      <c r="M27" s="8">
-        <v>43528</v>
-      </c>
-      <c r="N27" t="s">
-        <v>302</v>
-      </c>
-      <c r="O27">
-        <v>7136</v>
-      </c>
-      <c r="P27">
-        <v>494761</v>
-      </c>
-      <c r="Q27">
-        <v>1.44231255090842E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K28">
-        <v>20</v>
-      </c>
-      <c r="L28" t="s">
-        <v>382</v>
-      </c>
-      <c r="M28" t="s">
-        <v>25</v>
-      </c>
-      <c r="N28" t="s">
-        <v>302</v>
-      </c>
-      <c r="O28">
-        <v>835</v>
-      </c>
-      <c r="P28">
-        <v>494761</v>
-      </c>
-      <c r="Q28">
-        <v>1.6876835482182301E-3</v>
-      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3096,10 +2686,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,13 +2731,13 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>49884</v>
+        <v>49885</v>
       </c>
       <c r="E2">
         <v>52853</v>
       </c>
       <c r="F2">
-        <v>0.94382532684994203</v>
+        <v>0.94384424725181204</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3161,13 +2751,13 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>52853</v>
       </c>
       <c r="F3">
-        <v>6.6221406542675001E-4</v>
+        <v>6.8113446729608498E-4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3181,13 +2771,13 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>2494</v>
+        <v>2495</v>
       </c>
       <c r="E4">
         <v>52853</v>
       </c>
       <c r="F4">
-        <v>4.7187482262123201E-2</v>
+        <v>4.7206402663992598E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3201,13 +2791,13 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>52853</v>
       </c>
       <c r="F5" s="9">
-        <v>3.7840803738671399E-5</v>
+        <v>5.6761205608007102E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3221,13 +2811,13 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>52853</v>
       </c>
       <c r="F6">
-        <v>3.78408037386714E-4</v>
+        <v>3.9732843925605001E-4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3241,1033 +2831,1193 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E7">
         <v>52853</v>
       </c>
       <c r="F7">
-        <v>4.4841352430325604E-3</v>
+        <v>4.5030556449018998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>383</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>52853</v>
       </c>
-      <c r="F8">
-        <v>1.68391576637088E-3</v>
+      <c r="F8" s="9">
+        <v>1.89204018693357E-5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="E9">
         <v>52853</v>
       </c>
       <c r="F9">
-        <v>4.3516924299472098E-4</v>
+        <v>1.7028361682402101E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>52853</v>
       </c>
       <c r="F10">
-        <v>7.9465687851210001E-4</v>
+        <v>4.5408964486405698E-4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E11">
         <v>52853</v>
       </c>
       <c r="F11">
-        <v>3.0272642990937098E-4</v>
+        <v>8.1357728038143498E-4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E12">
         <v>52853</v>
       </c>
       <c r="F12">
-        <v>2.08124420562693E-4</v>
+        <v>3.2164683177870698E-4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>361</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>15145</v>
+        <v>12</v>
       </c>
       <c r="E13">
-        <v>16037</v>
+        <v>52853</v>
       </c>
       <c r="F13">
-        <v>0.94437862443100296</v>
+        <v>2.27044822432028E-4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>384</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>16037</v>
-      </c>
-      <c r="F14">
-        <v>9.3533703311093105E-4</v>
+        <v>52853</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1.89204018693357E-5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>362</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>361</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15">
-        <v>740</v>
+        <v>15146</v>
       </c>
       <c r="E15">
         <v>16037</v>
       </c>
       <c r="F15">
-        <v>4.6143293633472603E-2</v>
+        <v>0.94444098023321099</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E16">
         <v>16037</v>
       </c>
       <c r="F16">
-        <v>5.61202219866559E-4</v>
+        <v>9.976928353183259E-4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17">
-        <v>73</v>
+        <v>741</v>
       </c>
       <c r="E17">
         <v>16037</v>
       </c>
       <c r="F17">
-        <v>4.5519735611398602E-3</v>
+        <v>4.620564943568E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>385</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>16037</v>
       </c>
-      <c r="F18">
-        <v>1.1847602419405099E-3</v>
+      <c r="F18" s="9">
+        <v>6.2355802207395396E-5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>16037</v>
       </c>
       <c r="F19">
-        <v>9.976928353183259E-4</v>
+        <v>6.2355802207395396E-4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="E20">
         <v>16037</v>
       </c>
       <c r="F20">
-        <v>6.8591382428134903E-4</v>
+        <v>4.6143293633472597E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>386</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>16037</v>
       </c>
-      <c r="F21">
-        <v>3.1177901103697698E-4</v>
+      <c r="F21" s="9">
+        <v>6.2355802207395396E-5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>16037</v>
       </c>
       <c r="F22">
-        <v>2.4942320882958202E-4</v>
+        <v>1.2471160441479101E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>363</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>361</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D23">
-        <v>33004</v>
+        <v>17</v>
       </c>
       <c r="E23">
-        <v>34756</v>
+        <v>16037</v>
       </c>
       <c r="F23">
-        <v>0.94959143744964902</v>
+        <v>1.06004863752572E-3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E24">
-        <v>34756</v>
+        <v>16037</v>
       </c>
       <c r="F24">
-        <v>5.4666820117389801E-4</v>
+        <v>7.4826962648874497E-4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25">
-        <v>1434</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>34756</v>
+        <v>16037</v>
       </c>
       <c r="F25">
-        <v>4.12590631833352E-2</v>
+        <v>3.74134813244372E-4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>34756</v>
-      </c>
-      <c r="F26" s="9">
-        <v>2.8772010588099901E-5</v>
+        <v>16037</v>
+      </c>
+      <c r="F26">
+        <v>3.1177901103697698E-4</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>387</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>34756</v>
-      </c>
-      <c r="F27">
-        <v>2.87720105880999E-4</v>
+        <v>16037</v>
+      </c>
+      <c r="F27" s="9">
+        <v>6.2355802207395396E-5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>363</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>361</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28">
-        <v>161</v>
+        <v>33005</v>
       </c>
       <c r="E28">
         <v>34756</v>
       </c>
       <c r="F28">
-        <v>4.6322937046840802E-3</v>
+        <v>0.94962020946023695</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E29">
         <v>34756</v>
       </c>
       <c r="F29">
-        <v>1.72632063528599E-3</v>
+        <v>5.75440211761998E-4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>1435</v>
       </c>
       <c r="E30">
         <v>34756</v>
       </c>
-      <c r="F30" s="9">
-        <v>8.6316031764299705E-5</v>
+      <c r="F30">
+        <v>4.12878351939234E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <v>34756</v>
       </c>
-      <c r="F31">
-        <v>1.0645643917597E-3</v>
+      <c r="F31" s="9">
+        <v>5.7544021176199801E-5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E32">
         <v>34756</v>
       </c>
       <c r="F32">
-        <v>7.4807227529059698E-4</v>
+        <v>3.1649211646909899E-4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="E33">
         <v>34756</v>
       </c>
-      <c r="F33" s="9">
-        <v>2.8772010588099901E-5</v>
+      <c r="F33">
+        <v>4.6610657152721799E-3</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>364</v>
+        <v>388</v>
       </c>
       <c r="B34" t="s">
-        <v>361</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D34">
-        <v>43751</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>46299</v>
-      </c>
-      <c r="F34">
-        <v>0.944966413961425</v>
+        <v>34756</v>
+      </c>
+      <c r="F34" s="9">
+        <v>2.8772010588099901E-5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D35">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="E35">
-        <v>46299</v>
+        <v>34756</v>
       </c>
       <c r="F35">
-        <v>1.5551091816237901E-3</v>
+        <v>1.7550926458740901E-3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D36">
-        <v>1968</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>46299</v>
+        <v>34756</v>
       </c>
       <c r="F36">
-        <v>4.2506317631050297E-2</v>
+        <v>1.150880423524E-4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E37">
-        <v>46299</v>
+        <v>34756</v>
       </c>
       <c r="F37">
-        <v>9.28745761247543E-4</v>
+        <v>1.0933364023477999E-3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>232</v>
+        <v>27</v>
       </c>
       <c r="E38">
-        <v>46299</v>
+        <v>34756</v>
       </c>
       <c r="F38">
-        <v>5.0109073630099999E-3</v>
+        <v>7.7684428587869697E-4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39">
-        <v>46299</v>
+        <v>34756</v>
       </c>
       <c r="F39" s="9">
-        <v>6.4796215900991401E-5</v>
+        <v>5.7544021176199801E-5</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>389</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D40">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>46299</v>
-      </c>
-      <c r="F40">
-        <v>1.8574915224950899E-3</v>
+        <v>34756</v>
+      </c>
+      <c r="F40" s="9">
+        <v>2.8772010588099901E-5</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>361</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
       </c>
       <c r="D41">
-        <v>68</v>
+        <v>43752</v>
       </c>
       <c r="E41">
         <v>46299</v>
       </c>
       <c r="F41">
-        <v>1.4687142270891399E-3</v>
+        <v>0.94498801270005806</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
       </c>
       <c r="D42">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="E42">
         <v>46299</v>
       </c>
       <c r="F42">
-        <v>8.6394954534655202E-4</v>
+        <v>1.57670792025746E-3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
       <c r="D43">
-        <v>24</v>
+        <v>1969</v>
       </c>
       <c r="E43">
         <v>46299</v>
       </c>
       <c r="F43">
-        <v>5.18369727207931E-4</v>
+        <v>4.2527916369683998E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>390</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
       </c>
       <c r="D44">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>46299</v>
       </c>
-      <c r="F44">
-        <v>1.94388647702974E-4</v>
+      <c r="F44" s="9">
+        <v>2.15987386336638E-5</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E45">
         <v>46299</v>
       </c>
-      <c r="F45" s="9">
-        <v>6.4796215900991401E-5</v>
+      <c r="F45">
+        <v>9.5034449988120695E-4</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>365</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>361</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D46">
-        <v>476043</v>
+        <v>233</v>
       </c>
       <c r="E46">
-        <v>494761</v>
+        <v>46299</v>
       </c>
       <c r="F46">
-        <v>0.96216759202928304</v>
+        <v>5.0325061016436596E-3</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>366</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D47">
-        <v>161</v>
+        <v>4</v>
       </c>
       <c r="E47">
-        <v>494761</v>
-      </c>
-      <c r="F47">
-        <v>3.2540964223130002E-4</v>
+        <v>46299</v>
+      </c>
+      <c r="F47" s="9">
+        <v>8.6394954534655202E-5</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>367</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D48">
-        <v>15645</v>
+        <v>87</v>
       </c>
       <c r="E48">
-        <v>494761</v>
+        <v>46299</v>
       </c>
       <c r="F48">
-        <v>3.1621328277693699E-2</v>
+        <v>1.8790902611287501E-3</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>368</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="E49">
-        <v>494761</v>
-      </c>
-      <c r="F49" s="9">
-        <v>1.21270674123466E-5</v>
+        <v>46299</v>
+      </c>
+      <c r="F49">
+        <v>1.4903129657228001E-3</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>369</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D50">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="E50">
-        <v>494761</v>
+        <v>46299</v>
       </c>
       <c r="F50">
-        <v>2.0818132391194901E-4</v>
+        <v>8.8554828398021597E-4</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>370</v>
+        <v>73</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D51">
-        <v>1459</v>
+        <v>25</v>
       </c>
       <c r="E51">
-        <v>494761</v>
+        <v>46299</v>
       </c>
       <c r="F51">
-        <v>2.9488985591022698E-3</v>
+        <v>5.3996846584159505E-4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>371</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D52">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E52">
-        <v>494761</v>
-      </c>
-      <c r="F52" s="9">
-        <v>1.8190601118519799E-5</v>
+        <v>46299</v>
+      </c>
+      <c r="F52">
+        <v>2.15987386336638E-4</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>372</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>302</v>
+        <v>13</v>
       </c>
       <c r="D53">
-        <v>642</v>
+        <v>4</v>
       </c>
       <c r="E53">
-        <v>494761</v>
-      </c>
-      <c r="F53">
-        <v>1.2975962131210801E-3</v>
+        <v>46299</v>
+      </c>
+      <c r="F53" s="9">
+        <v>8.6394954534655202E-5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>361</v>
       </c>
       <c r="C54" t="s">
         <v>302</v>
       </c>
       <c r="D54">
-        <v>135</v>
+        <v>476044</v>
       </c>
       <c r="E54">
         <v>494761</v>
       </c>
       <c r="F54">
-        <v>2.7285901677779798E-4</v>
+        <v>0.96216961320718497</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
         <v>302</v>
       </c>
       <c r="D55">
-        <v>336</v>
+        <v>162</v>
       </c>
       <c r="E55">
         <v>494761</v>
       </c>
       <c r="F55">
-        <v>6.7911577509140804E-4</v>
+        <v>3.2743082013335698E-4</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C56" t="s">
         <v>302</v>
       </c>
       <c r="D56">
-        <v>140</v>
+        <v>15646</v>
       </c>
       <c r="E56">
         <v>494761</v>
       </c>
       <c r="F56">
-        <v>2.8296490628808703E-4</v>
+        <v>3.1623349455595702E-2</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
         <v>302</v>
       </c>
       <c r="D57">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="E57">
         <v>494761</v>
       </c>
-      <c r="F57">
-        <v>1.49567164752274E-4</v>
+      <c r="F57" s="9">
+        <v>1.4148245314404299E-5</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C58" t="s">
         <v>302</v>
       </c>
       <c r="D58">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="E58">
         <v>494761</v>
       </c>
-      <c r="F58" s="9">
-        <v>1.61694232164621E-5</v>
+      <c r="F58">
+        <v>2.1020250181400701E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>370</v>
+      </c>
+      <c r="B59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" t="s">
+        <v>302</v>
+      </c>
+      <c r="D59">
+        <v>1460</v>
+      </c>
+      <c r="E59">
+        <v>494761</v>
+      </c>
+      <c r="F59">
+        <v>2.9509197370043302E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" t="s">
+        <v>302</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>494761</v>
+      </c>
+      <c r="F60" s="9">
+        <v>2.0211779020577599E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>372</v>
+      </c>
+      <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D61">
+        <v>643</v>
+      </c>
+      <c r="E61">
+        <v>494761</v>
+      </c>
+      <c r="F61">
+        <v>1.29961739102314E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>373</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" t="s">
+        <v>302</v>
+      </c>
+      <c r="D62">
+        <v>136</v>
+      </c>
+      <c r="E62">
+        <v>494761</v>
+      </c>
+      <c r="F62">
+        <v>2.7488019467985597E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>374</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" t="s">
+        <v>302</v>
+      </c>
+      <c r="D63">
+        <v>337</v>
+      </c>
+      <c r="E63">
+        <v>494761</v>
+      </c>
+      <c r="F63">
+        <v>6.8113695299346598E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>375</v>
+      </c>
+      <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" t="s">
+        <v>302</v>
+      </c>
+      <c r="D64">
+        <v>141</v>
+      </c>
+      <c r="E64">
+        <v>494761</v>
+      </c>
+      <c r="F64">
+        <v>2.8498608419014399E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>376</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" t="s">
+        <v>302</v>
+      </c>
+      <c r="D65">
+        <v>75</v>
+      </c>
+      <c r="E65">
+        <v>494761</v>
+      </c>
+      <c r="F65">
+        <v>1.5158834265433199E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>377</v>
+      </c>
+      <c r="B66" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" t="s">
+        <v>302</v>
+      </c>
+      <c r="D66">
+        <v>9</v>
+      </c>
+      <c r="E66">
+        <v>494761</v>
+      </c>
+      <c r="F66" s="9">
+        <v>1.8190601118519799E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>